<commit_message>
versione del 24 ottobre
</commit_message>
<xml_diff>
--- a/b_df.xlsx
+++ b/b_df.xlsx
@@ -489,7 +489,7 @@
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198A8354190&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E782C03090&gt;</t>
         </is>
       </c>
       <c r="D2" t="n">
@@ -502,13 +502,13 @@
         <v>0</v>
       </c>
       <c r="G2" t="n">
-        <v>8.092944235783254</v>
+        <v>4.558594024346748</v>
       </c>
       <c r="H2" t="n">
-        <v>10.57</v>
+        <v>3.5</v>
       </c>
       <c r="I2" t="n">
-        <v>26.21641402471921</v>
+        <v>7.549857829483546</v>
       </c>
       <c r="J2" t="n">
         <v>10.96405234596766</v>
@@ -523,7 +523,7 @@
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198B2724390&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E7804AFF50&gt;</t>
         </is>
       </c>
       <c r="D3" t="n">
@@ -536,13 +536,13 @@
         <v>0</v>
       </c>
       <c r="G3" t="n">
-        <v>20.83894641170696</v>
+        <v>9.994117823433328</v>
       </c>
       <c r="H3" t="n">
         <v>10.57</v>
       </c>
       <c r="I3" t="n">
-        <v>7.421459665928201</v>
+        <v>13.35831707259888</v>
       </c>
       <c r="J3" t="n">
         <v>9.600157208367223</v>
@@ -557,7 +557,7 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198A9965F10&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E782DA9390&gt;</t>
         </is>
       </c>
       <c r="D4" t="n">
@@ -570,13 +570,13 @@
         <v>0</v>
       </c>
       <c r="G4" t="n">
-        <v>4.262921281204147</v>
+        <v>20.86020829870003</v>
       </c>
       <c r="H4" t="n">
         <v>10.57</v>
       </c>
       <c r="I4" t="n">
-        <v>14.22225237810268</v>
+        <v>8.545549680531575</v>
       </c>
       <c r="J4" t="n">
         <v>10.17873798410574</v>
@@ -591,7 +591,7 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198B20658D0&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E780309FD0&gt;</t>
         </is>
       </c>
       <c r="D5" t="n">
@@ -604,13 +604,13 @@
         <v>0</v>
       </c>
       <c r="G5" t="n">
-        <v>16.10884698466955</v>
+        <v>31.30957989156325</v>
       </c>
       <c r="H5" t="n">
         <v>10.57</v>
       </c>
       <c r="I5" t="n">
-        <v>8.758682382049395</v>
+        <v>41.81996940997271</v>
       </c>
       <c r="J5" t="n">
         <v>11.44089319920146</v>
@@ -625,7 +625,7 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198B2725690&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E782CA2010&gt;</t>
         </is>
       </c>
       <c r="D6" t="n">
@@ -638,13 +638,13 @@
         <v>0</v>
       </c>
       <c r="G6" t="n">
-        <v>5.235865470440293</v>
+        <v>4.692896436942904</v>
       </c>
       <c r="H6" t="n">
         <v>10.57</v>
       </c>
       <c r="I6" t="n">
-        <v>9.957885562123209</v>
+        <v>11.01765782958361</v>
       </c>
       <c r="J6" t="n">
         <v>11.06755799014997</v>
@@ -659,7 +659,7 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198AA8ED390&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E780221710&gt;</t>
         </is>
       </c>
       <c r="D7" t="n">
@@ -672,13 +672,13 @@
         <v>0</v>
       </c>
       <c r="G7" t="n">
-        <v>5.689572361914922</v>
+        <v>11.511948905071</v>
       </c>
       <c r="H7" t="n">
-        <v>10.57</v>
+        <v>3.5</v>
       </c>
       <c r="I7" t="n">
-        <v>13.24500386671677</v>
+        <v>9.092649555729189</v>
       </c>
       <c r="J7" t="n">
         <v>8.222722120123588</v>
@@ -693,7 +693,7 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198AA8EFA90&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E780223550&gt;</t>
         </is>
       </c>
       <c r="D8" t="n">
@@ -706,13 +706,13 @@
         <v>0</v>
       </c>
       <c r="G8" t="n">
-        <v>6.624710756998347</v>
+        <v>4.449041314942946</v>
       </c>
       <c r="H8" t="n">
-        <v>10.57</v>
+        <v>3.5</v>
       </c>
       <c r="I8" t="n">
-        <v>6.740510347676921</v>
+        <v>4.152982905834425</v>
       </c>
       <c r="J8" t="n">
         <v>10.15008841752559</v>
@@ -727,7 +727,7 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198AA8ECD50&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E780221750&gt;</t>
         </is>
       </c>
       <c r="D9" t="n">
@@ -740,13 +740,13 @@
         <v>0</v>
       </c>
       <c r="G9" t="n">
-        <v>9.815751870894772</v>
+        <v>14.58877561852719</v>
       </c>
       <c r="H9" t="n">
         <v>10.57</v>
       </c>
       <c r="I9" t="n">
-        <v>19.37815964314971</v>
+        <v>23.69276483116812</v>
       </c>
       <c r="J9" t="n">
         <v>9.048642791702301</v>
@@ -761,7 +761,7 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198AA8EFAD0&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E78041D4D0&gt;</t>
         </is>
       </c>
       <c r="D10" t="n">
@@ -774,13 +774,13 @@
         <v>0</v>
       </c>
       <c r="G10" t="n">
-        <v>5.309141009743146</v>
+        <v>11.98991920880145</v>
       </c>
       <c r="H10" t="n">
         <v>10.57</v>
       </c>
       <c r="I10" t="n">
-        <v>26.87143188381797</v>
+        <v>11.75015264334031</v>
       </c>
       <c r="J10" t="n">
         <v>9.096781148206441</v>
@@ -795,7 +795,7 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>&lt;__main__.Entity object at 0x00000198AA8ED7D0&gt;</t>
+          <t>&lt;__main__.Entity object at 0x000001E782A8FE50&gt;</t>
         </is>
       </c>
       <c r="D11" t="n">
@@ -808,13 +808,13 @@
         <v>0</v>
       </c>
       <c r="G11" t="n">
-        <v>3.972212280205519</v>
+        <v>6.647026366299166</v>
       </c>
       <c r="H11" t="n">
         <v>10.57</v>
       </c>
       <c r="I11" t="n">
-        <v>9.547133088722376</v>
+        <v>4.131813628053326</v>
       </c>
       <c r="J11" t="n">
         <v>9.610598501938371</v>

</xml_diff>